<commit_message>
Proceso de Gestion Cambios a Requerimientos
Proceso de Gestion Cambios a Requerimientos
</commit_message>
<xml_diff>
--- a/Importante.xlsx
+++ b/Importante.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\GitHub\UTP-GPS-ALARM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Perochena\Documents\GitHub\UTP-GPS-ALARM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1548,57 +1548,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1632,9 +1581,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1650,13 +1596,67 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Cancel" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="55">
     <dxf>
       <fill>
         <patternFill>
@@ -2039,293 +2039,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2679,10 +2392,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2698,79 +2411,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="87"/>
-      <c r="K1" s="83" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="106"/>
+      <c r="K1" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="90"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="109"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="90"/>
-      <c r="K3" s="84" t="s">
+      <c r="B3" s="107"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="109"/>
+      <c r="K3" s="103" t="s">
         <v>138</v>
       </c>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
-      <c r="B4" s="88"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="90"/>
-      <c r="K4" s="84" t="s">
+      <c r="B4" s="107"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="109"/>
+      <c r="K4" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B5" s="91"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="93"/>
-      <c r="K5" s="84" t="s">
-        <v>139</v>
-      </c>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="112"/>
+      <c r="K5" s="103" t="s">
+        <v>139</v>
+      </c>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
     </row>
     <row r="6" spans="1:13" ht="30.75" thickBot="1">
       <c r="A6" s="15" t="s">
@@ -2802,12 +2515,12 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="101"/>
     </row>
     <row r="8" spans="1:13" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A8" s="37">
@@ -2867,32 +2580,32 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="97" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="10" spans="1:13" s="80" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A10" s="37">
         <v>3</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="100" t="s">
+      <c r="D10" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="G10" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="H10" s="98" t="s">
+      <c r="E10" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="I10" s="98" t="s">
+      <c r="I10" s="81" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2954,72 +2667,72 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="102" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A13" s="109">
+    <row r="13" spans="1:13" s="85" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A13" s="92">
         <v>6</v>
       </c>
-      <c r="B13" s="102" t="s">
+      <c r="B13" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="101" t="s">
-        <v>139</v>
-      </c>
-      <c r="F13" s="101" t="s">
-        <v>139</v>
-      </c>
-      <c r="G13" s="101" t="s">
-        <v>139</v>
-      </c>
-      <c r="H13" s="101" t="s">
+      <c r="E13" s="84" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="84" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="84" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="84" t="s">
         <v>138</v>
       </c>
-      <c r="I13" s="101" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="97" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="I13" s="84" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="80" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A14" s="37">
         <v>7</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="100" t="s">
+      <c r="D14" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="F14" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="G14" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="H14" s="98" t="s">
+      <c r="E14" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="I14" s="98" t="s">
+      <c r="I14" s="81" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16.5" thickTop="1" thickBot="1"/>
     <row r="16" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="82"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="101"/>
     </row>
     <row r="17" spans="1:16" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A17" s="37">
@@ -3201,11 +2914,11 @@
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:16" ht="19.5" thickBot="1">
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="95"/>
-      <c r="D24" s="96"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="115"/>
     </row>
     <row r="25" spans="1:16" s="38" customFormat="1" ht="15.75" thickBot="1">
       <c r="A25" s="37">
@@ -3217,7 +2930,7 @@
       <c r="C25" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="108" t="s">
+      <c r="D25" s="91" t="s">
         <v>73</v>
       </c>
       <c r="E25" s="37" t="s">
@@ -3266,16 +2979,16 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A27" s="109">
+      <c r="A27" s="92">
         <v>3</v>
       </c>
-      <c r="B27" s="105" t="s">
+      <c r="B27" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="107" t="s">
+      <c r="D27" s="90" t="s">
         <v>87</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -3294,75 +3007,75 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="105" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A28" s="109">
+    <row r="28" spans="1:16" s="88" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A28" s="92">
         <v>4</v>
       </c>
-      <c r="B28" s="105" t="s">
+      <c r="B28" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="107" t="s">
+      <c r="D28" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="F28" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="G28" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="H28" s="109" t="s">
+      <c r="E28" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="G28" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="92" t="s">
         <v>138</v>
       </c>
-      <c r="I28" s="109" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="105" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A29" s="109">
+      <c r="I28" s="92" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="88" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A29" s="92">
         <v>5</v>
       </c>
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="107" t="s">
+      <c r="D29" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="F29" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="G29" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="109" t="s">
+      <c r="E29" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="92" t="s">
         <v>138</v>
       </c>
-      <c r="I29" s="109" t="s">
+      <c r="I29" s="92" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="24.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A30" s="109">
+      <c r="A30" s="92">
         <v>6</v>
       </c>
-      <c r="B30" s="105" t="s">
+      <c r="B30" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="106" t="s">
+      <c r="C30" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="107" t="s">
+      <c r="D30" s="90" t="s">
         <v>89</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -3380,25 +3093,25 @@
       <c r="I30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J30" s="110" t="s">
+      <c r="J30" s="116" t="s">
         <v>213</v>
       </c>
-      <c r="K30" s="110"/>
-      <c r="L30" s="110"/>
-      <c r="M30" s="110"/>
-      <c r="N30" s="110"/>
-      <c r="O30" s="110"/>
-      <c r="P30" s="110"/>
+      <c r="K30" s="116"/>
+      <c r="L30" s="116"/>
+      <c r="M30" s="116"/>
+      <c r="N30" s="116"/>
+      <c r="O30" s="116"/>
+      <c r="P30" s="116"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" thickTop="1"/>
     <row r="32" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="33" spans="1:9" ht="29.25" thickBot="1">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
+      <c r="D33" s="101"/>
     </row>
     <row r="34" spans="1:9" s="38" customFormat="1" ht="15.75" thickBot="1">
       <c r="A34" s="37">
@@ -3487,44 +3200,44 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="97" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A37" s="98">
+    <row r="37" spans="1:9" s="80" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A37" s="81">
         <v>6</v>
       </c>
-      <c r="B37" s="97" t="s">
+      <c r="B37" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="111" t="s">
+      <c r="C37" s="93" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="112" t="s">
+      <c r="D37" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="F37" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="G37" s="98" t="s">
-        <v>139</v>
-      </c>
-      <c r="H37" s="98" t="s">
+      <c r="E37" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" s="81" t="s">
+        <v>139</v>
+      </c>
+      <c r="H37" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="I37" s="98" t="s">
+      <c r="I37" s="81" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickTop="1"/>
     <row r="40" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="41" spans="1:9" ht="29.25" thickBot="1">
-      <c r="A41" s="80" t="s">
+      <c r="A41" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="82"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="101"/>
     </row>
     <row r="42" spans="1:9" s="38" customFormat="1" ht="15.75" thickBot="1">
       <c r="A42" s="37">
@@ -3642,32 +3355,32 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="105" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A46" s="114">
+    <row r="46" spans="1:9" s="88" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A46" s="96">
         <v>6</v>
       </c>
-      <c r="B46" s="115" t="s">
+      <c r="B46" s="97" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="113" t="s">
+      <c r="C46" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="107" t="s">
+      <c r="D46" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="E46" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" s="109" t="s">
-        <v>139</v>
-      </c>
-      <c r="H46" s="109" t="s">
+      <c r="E46" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="H46" s="92" t="s">
         <v>138</v>
       </c>
-      <c r="I46" s="109" t="s">
+      <c r="I46" s="92" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3675,12 +3388,12 @@
       <c r="C47" s="22"/>
     </row>
     <row r="48" spans="1:9" ht="29.25" thickBot="1">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="82"/>
+      <c r="B48" s="100"/>
+      <c r="C48" s="100"/>
+      <c r="D48" s="101"/>
     </row>
     <row r="49" spans="1:9" s="38" customFormat="1">
       <c r="A49" s="37">
@@ -3744,7 +3457,7 @@
       <c r="A51" s="37">
         <v>3</v>
       </c>
-      <c r="B51" s="116" t="s">
+      <c r="B51" s="98" t="s">
         <v>204</v>
       </c>
       <c r="C51" s="37" t="s">
@@ -3773,7 +3486,7 @@
       <c r="A52" s="37">
         <v>4</v>
       </c>
-      <c r="B52" s="116" t="s">
+      <c r="B52" s="98" t="s">
         <v>207</v>
       </c>
       <c r="C52" s="37" t="s">
@@ -3802,7 +3515,7 @@
       <c r="A53" s="37">
         <v>5</v>
       </c>
-      <c r="B53" s="116" t="s">
+      <c r="B53" s="98" t="s">
         <v>210</v>
       </c>
       <c r="C53" s="37" t="s">
@@ -3831,7 +3544,7 @@
       <c r="A54" s="37">
         <v>6</v>
       </c>
-      <c r="B54" s="116" t="s">
+      <c r="B54" s="98" t="s">
         <v>214</v>
       </c>
       <c r="C54" s="37" t="s">
@@ -3858,28 +3571,112 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="56" spans="1:9" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A56" s="80" t="s">
+      <c r="A56" s="99" t="s">
         <v>217</v>
       </c>
-      <c r="B56" s="81"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="82"/>
-    </row>
-    <row r="57" spans="1:9" s="58" customFormat="1"/>
-    <row r="58" spans="1:9" s="58" customFormat="1"/>
-    <row r="59" spans="1:9" s="58" customFormat="1" ht="15.75" thickBot="1"/>
-    <row r="60" spans="1:9" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B56" s="100"/>
+      <c r="C56" s="100"/>
+      <c r="D56" s="101"/>
+    </row>
+    <row r="57" spans="1:9" s="38" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A57" s="37">
+        <v>4</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="F57" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="H57" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I57" s="37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A58" s="37">
+        <v>6</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="G58" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="H58" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I58" s="37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A59" s="37">
+        <v>7</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E59" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="F59" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="G59" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="H59" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="I59" s="37" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A60" s="37">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D60" s="44" t="s">
-        <v>126</v>
+        <v>58</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="E60" s="37" t="s">
         <v>139</v>
@@ -3897,94 +3694,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A61" s="37">
-        <v>6</v>
-      </c>
-      <c r="B61" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="E61" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="F61" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="G61" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="H61" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="I61" s="37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A62" s="37">
-        <v>7</v>
-      </c>
-      <c r="B62" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="E62" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="F62" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="G62" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="H62" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="I62" s="37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A63" s="37">
-        <v>9</v>
-      </c>
-      <c r="B63" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D63" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E63" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="F63" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="G63" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="H63" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="I63" s="37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.75" thickTop="1"/>
+    <row r="61" spans="1:9" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A33:D33"/>
@@ -4001,17 +3711,17 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="J30:P30"/>
   </mergeCells>
-  <conditionalFormatting sqref="G8:G14 G61:G63 I8:I14 I61:I63">
+  <conditionalFormatting sqref="G8:G14 G58:G60 I8:I14 I58:I60">
     <cfRule type="expression" dxfId="54" priority="28">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G14 G61:G63 I8:I14 I61:I63">
+  <conditionalFormatting sqref="G8:G14 G58:G60 I8:I14 I58:I60">
     <cfRule type="cellIs" dxfId="53" priority="27" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34:G37 E8:I14 E61:I63">
+  <conditionalFormatting sqref="E34:G37 E8:I14 E58:I60">
     <cfRule type="cellIs" dxfId="52" priority="21" operator="equal">
       <formula>"REVISAR"</formula>
     </cfRule>
@@ -4022,7 +3732,7 @@
       <formula>NOT(ISERROR(SEARCH("SI",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23:I24 H17:I22 E31:I33 H25:I30 E38:I41 E47:I48 E55:I56 E64:I101 H60:I60 H34:I37 H42:I46 H49:I54">
+  <conditionalFormatting sqref="E23:I24 H17:I22 E31:I33 H25:I30 E38:I41 E47:I48 E55:I56 E61:I98 H57:I57 H34:I37 H42:I46 H49:I54">
     <cfRule type="cellIs" dxfId="49" priority="22" operator="equal">
       <formula>"REVISAR"</formula>
     </cfRule>
@@ -4077,7 +3787,7 @@
       <formula>NOT(ISERROR(SEARCH("SI",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E60:G60">
+  <conditionalFormatting sqref="E57:G57">
     <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>"REVISAR"</formula>
     </cfRule>
@@ -4085,7 +3795,7 @@
       <formula>"NO"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="32" priority="5" operator="containsText" text="SI">
-      <formula>NOT(ISERROR(SEARCH("SI",E60)))</formula>
+      <formula>NOT(ISERROR(SEARCH("SI",E57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4114,12 +3824,12 @@
   <sheetData>
     <row r="3" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:5" ht="29.25" thickBot="1">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="82"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="101"/>
     </row>
     <row r="19" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="20" spans="2:11" ht="16.5" thickTop="1" thickBot="1">

</xml_diff>